<commit_message>
add path, query and body to system spec
</commit_message>
<xml_diff>
--- a/adhafera/test/system_spec.xlsx
+++ b/adhafera/test/system_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="130">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -876,6 +876,293 @@
     <rPh sb="27" eb="28">
       <t>カエ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Query</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Body</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/[:table]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date, content, category, price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/[:table]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: date
+with: *</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: content
+with: *</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: category
+with: *</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: price
+with: *</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: [date, content, category, price]{2,4}
+with: *</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[date, content, category, price]{2,4}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: -
+with: *</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: *
+with: date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: *
+with: content</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: *
+with: category</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: *
+with: price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: *
+with: [date, content, category, price]{2,4}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[date, content, category, price]{2,4}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/settlement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/settlement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>period=monthly</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>period=weekly</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>period=daily</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Query</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Body</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/[:table]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>content, category, price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date, category, price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date, content, price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date, content, category</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[date, content, category, price]{1,2}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>invalid_date, content, category, price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date, content, category, invalid_price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>invalid_date, content, category, invalid_price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date=invalid_date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>price=invalid_price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>period=invalid_period</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: invalid_date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: invalid_price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>with: invalid_date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>with: invalid_price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>with: -</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>invalid_date, content, category, price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date, content, category, invalid_price</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -932,7 +1219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1321,6 +1608,89 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1351,7 +1721,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1438,6 +1808,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="25">
@@ -1794,19 +2201,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E29"/>
+  <dimension ref="B1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="5" width="70.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="7" width="40.1640625" customWidth="1"/>
+    <col min="8" max="8" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="19" thickBot="1"/>
-    <row r="2" spans="2:5" ht="19" thickBot="1">
+    <row r="1" spans="2:8" ht="19" thickBot="1"/>
+    <row r="2" spans="2:8" ht="19" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1816,11 +2227,20 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="31">
+    <row r="3" spans="2:8" ht="31">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -1830,11 +2250,20 @@
       <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="31">
+    <row r="4" spans="2:8" ht="31">
       <c r="B4" s="13">
         <v>2</v>
       </c>
@@ -1844,11 +2273,20 @@
       <c r="D4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="31">
+    <row r="5" spans="2:8" ht="31">
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -1858,11 +2296,20 @@
       <c r="D5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="31">
+    <row r="6" spans="2:8" ht="31">
       <c r="B6" s="17">
         <v>4</v>
       </c>
@@ -1872,11 +2319,20 @@
       <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="31">
+    <row r="7" spans="2:8" ht="31">
       <c r="B7" s="17">
         <v>5</v>
       </c>
@@ -1886,11 +2342,20 @@
       <c r="D7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="31">
+    <row r="8" spans="2:8" ht="31">
       <c r="B8" s="17">
         <v>6</v>
       </c>
@@ -1900,11 +2365,20 @@
       <c r="D8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="31">
+    <row r="9" spans="2:8" ht="31">
       <c r="B9" s="17">
         <v>7</v>
       </c>
@@ -1914,11 +2388,20 @@
       <c r="D9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="31">
+    <row r="10" spans="2:8" ht="31">
       <c r="B10" s="17">
         <v>8</v>
       </c>
@@ -1928,11 +2411,20 @@
       <c r="D10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="31">
+    <row r="11" spans="2:8" ht="31">
       <c r="B11" s="17">
         <v>9</v>
       </c>
@@ -1942,11 +2434,20 @@
       <c r="D11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="31">
+    <row r="12" spans="2:8" ht="31">
       <c r="B12" s="17">
         <v>10</v>
       </c>
@@ -1956,11 +2457,20 @@
       <c r="D12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="31">
+    <row r="13" spans="2:8" ht="31">
       <c r="B13" s="17">
         <v>11</v>
       </c>
@@ -1970,11 +2480,20 @@
       <c r="D13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="31">
+    <row r="14" spans="2:8" ht="31">
       <c r="B14" s="17">
         <v>12</v>
       </c>
@@ -1984,11 +2503,20 @@
       <c r="D14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="31">
+    <row r="15" spans="2:8" ht="31">
       <c r="B15" s="17">
         <v>13</v>
       </c>
@@ -1998,11 +2526,20 @@
       <c r="D15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="31">
+    <row r="16" spans="2:8" ht="31">
       <c r="B16" s="21">
         <v>14</v>
       </c>
@@ -2012,11 +2549,20 @@
       <c r="D16" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="31">
+    <row r="17" spans="2:8" ht="31">
       <c r="B17" s="21">
         <v>15</v>
       </c>
@@ -2026,11 +2572,20 @@
       <c r="D17" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="31">
+    <row r="18" spans="2:8" ht="31">
       <c r="B18" s="21">
         <v>16</v>
       </c>
@@ -2040,11 +2595,20 @@
       <c r="D18" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="31">
+    <row r="19" spans="2:8" ht="31">
       <c r="B19" s="21">
         <v>17</v>
       </c>
@@ -2054,11 +2618,20 @@
       <c r="D19" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="31">
+    <row r="20" spans="2:8" ht="31">
       <c r="B20" s="21">
         <v>18</v>
       </c>
@@ -2068,11 +2641,20 @@
       <c r="D20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:8">
       <c r="B21" s="21">
         <v>19</v>
       </c>
@@ -2082,11 +2664,20 @@
       <c r="D21" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:8">
       <c r="B22" s="21">
         <v>20</v>
       </c>
@@ -2096,11 +2687,20 @@
       <c r="D22" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:8">
       <c r="B23" s="21">
         <v>21</v>
       </c>
@@ -2110,11 +2710,20 @@
       <c r="D23" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:8">
       <c r="B24" s="21">
         <v>22</v>
       </c>
@@ -2124,11 +2733,20 @@
       <c r="D24" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:8">
       <c r="B25" s="21">
         <v>23</v>
       </c>
@@ -2138,11 +2756,20 @@
       <c r="D25" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:8">
       <c r="B26" s="21">
         <v>24</v>
       </c>
@@ -2152,11 +2779,20 @@
       <c r="D26" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="31">
+    <row r="27" spans="2:8" ht="31">
       <c r="B27" s="21">
         <v>25</v>
       </c>
@@ -2166,11 +2802,20 @@
       <c r="D27" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="31">
+    <row r="28" spans="2:8" ht="31">
       <c r="B28" s="21">
         <v>26</v>
       </c>
@@ -2180,11 +2825,20 @@
       <c r="D28" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="32" thickBot="1">
+    <row r="29" spans="2:8" ht="32" thickBot="1">
       <c r="B29" s="11">
         <v>27</v>
       </c>
@@ -2194,7 +2848,16 @@
       <c r="D29" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2212,19 +2875,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E22"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="5" width="70.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="7" width="40.1640625" customWidth="1"/>
+    <col min="8" max="8" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="19" thickBot="1"/>
-    <row r="2" spans="2:5" ht="19" thickBot="1">
+    <row r="1" spans="2:8" ht="19" thickBot="1"/>
+    <row r="2" spans="2:8" ht="19" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2234,11 +2901,20 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="31">
+    <row r="3" spans="2:8" ht="31">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -2248,11 +2924,20 @@
       <c r="D3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="31">
+    <row r="4" spans="2:8" ht="31">
       <c r="B4" s="27">
         <v>2</v>
       </c>
@@ -2262,11 +2947,20 @@
       <c r="D4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="31">
+    <row r="5" spans="2:8" ht="31">
       <c r="B5" s="27">
         <v>3</v>
       </c>
@@ -2276,11 +2970,20 @@
       <c r="D5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="31">
+    <row r="6" spans="2:8" ht="31">
       <c r="B6" s="27">
         <v>4</v>
       </c>
@@ -2290,11 +2993,20 @@
       <c r="D6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="31">
+    <row r="7" spans="2:8" ht="31">
       <c r="B7" s="27">
         <v>5</v>
       </c>
@@ -2304,11 +3016,20 @@
       <c r="D7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="31">
+    <row r="8" spans="2:8" ht="31">
       <c r="B8" s="27">
         <v>6</v>
       </c>
@@ -2318,11 +3039,20 @@
       <c r="D8" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="31">
+    <row r="9" spans="2:8" ht="31">
       <c r="B9" s="17">
         <v>7</v>
       </c>
@@ -2332,11 +3062,20 @@
       <c r="D9" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="31">
+    <row r="10" spans="2:8" ht="31">
       <c r="B10" s="17">
         <v>8</v>
       </c>
@@ -2346,11 +3085,20 @@
       <c r="D10" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="31">
+    <row r="11" spans="2:8" ht="31">
       <c r="B11" s="17">
         <v>9</v>
       </c>
@@ -2360,11 +3108,20 @@
       <c r="D11" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="31">
+    <row r="12" spans="2:8" ht="31">
       <c r="B12" s="17">
         <v>10</v>
       </c>
@@ -2374,11 +3131,20 @@
       <c r="D12" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="31">
+    <row r="13" spans="2:8" ht="31">
       <c r="B13" s="17">
         <v>11</v>
       </c>
@@ -2388,11 +3154,20 @@
       <c r="D13" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="31">
+    <row r="14" spans="2:8" ht="31">
       <c r="B14" s="17">
         <v>12</v>
       </c>
@@ -2402,11 +3177,20 @@
       <c r="D14" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="31">
+    <row r="15" spans="2:8" ht="31">
       <c r="B15" s="17">
         <v>13</v>
       </c>
@@ -2416,11 +3200,20 @@
       <c r="D15" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="31">
+    <row r="16" spans="2:8" ht="31">
       <c r="B16" s="17">
         <v>14</v>
       </c>
@@ -2430,11 +3223,20 @@
       <c r="D16" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="31">
+    <row r="17" spans="2:8" ht="31">
       <c r="B17" s="17">
         <v>15</v>
       </c>
@@ -2444,11 +3246,20 @@
       <c r="D17" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="31">
+    <row r="18" spans="2:8" ht="31">
       <c r="B18" s="17">
         <v>16</v>
       </c>
@@ -2458,11 +3269,20 @@
       <c r="D18" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="31">
+    <row r="19" spans="2:8" ht="31">
       <c r="B19" s="17">
         <v>17</v>
       </c>
@@ -2472,11 +3292,20 @@
       <c r="D19" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="31">
+    <row r="20" spans="2:8" ht="31">
       <c r="B20" s="17">
         <v>18</v>
       </c>
@@ -2486,11 +3315,20 @@
       <c r="D20" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="32" thickBot="1">
+    <row r="21" spans="2:8" ht="32" thickBot="1">
       <c r="B21" s="21">
         <v>19</v>
       </c>
@@ -2500,15 +3338,27 @@
       <c r="D21" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:8">
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>